<commit_message>
updated LLBv3 pin mapping document; matches current state of board
</commit_message>
<xml_diff>
--- a/Electronics/Low Level v3/Pin Mapping.xlsx
+++ b/Electronics/Low Level v3/Pin Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5A656D-A1A5-694F-9EFE-4BA0819D2785}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F535DA3-0721-434A-900B-D42314399404}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="21160" xr2:uid="{2E9AF3F1-2BA1-F14D-8C1F-E5BC4609F5C6}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="214">
   <si>
     <t>PG5 ( OC0B )</t>
   </si>
@@ -536,9 +536,6 @@
     <t>LLBV3 Pin Name</t>
   </si>
   <si>
-    <t>LLBV3 Header</t>
-  </si>
-  <si>
     <t>RX3</t>
   </si>
   <si>
@@ -645,6 +642,36 @@
   </si>
   <si>
     <t>R_RTN_GND</t>
+  </si>
+  <si>
+    <t>LLBV3 Header / Function</t>
+  </si>
+  <si>
+    <t>MCP 2515 interrupt on received frames</t>
+  </si>
+  <si>
+    <t>E-stop jumper, also X3</t>
+  </si>
+  <si>
+    <t>wheel hall switch header</t>
+  </si>
+  <si>
+    <t>all SPI devices, SPI header</t>
+  </si>
+  <si>
+    <t>SPI header (this pin tells the mega to be a slave)</t>
+  </si>
+  <si>
+    <t>MCP2515 slave selection</t>
+  </si>
+  <si>
+    <t>DAC slave selection</t>
+  </si>
+  <si>
+    <t>on-board buzzer</t>
+  </si>
+  <si>
+    <t>X3, no purpose assgined</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4080FD99-07AF-0640-A5AF-54DF0F777A9D}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,7 +1135,7 @@
         <v>167</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1122,7 +1149,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1136,10 +1166,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1153,10 +1183,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" t="s">
         <v>173</v>
-      </c>
-      <c r="E4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1179,7 +1209,10 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>183</v>
+      </c>
+      <c r="E6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1193,7 +1226,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1207,7 +1243,10 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1303,10 +1342,10 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" t="s">
         <v>185</v>
-      </c>
-      <c r="E17" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1320,7 +1359,10 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="E18" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1334,7 +1376,10 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="E19" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1348,7 +1393,10 @@
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>174</v>
+      </c>
+      <c r="E20" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,7 +1410,10 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="E21" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1376,7 +1427,10 @@
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>197</v>
+        <v>196</v>
+      </c>
+      <c r="E22" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1390,7 +1444,10 @@
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+      <c r="E23" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1404,10 +1461,10 @@
         <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1421,10 +1478,10 @@
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1438,10 +1495,10 @@
         <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1455,10 +1512,10 @@
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1510,7 +1567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1521,7 +1578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1532,7 +1589,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1543,7 +1600,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1554,10 +1611,13 @@
         <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+      <c r="E36" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -1568,10 +1628,13 @@
         <v>55</v>
       </c>
       <c r="D37" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+      <c r="E37" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1582,7 +1645,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -1593,7 +1656,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -1604,7 +1667,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -1615,7 +1678,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -1626,7 +1689,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -1637,7 +1700,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -1648,7 +1711,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -1659,7 +1722,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -1670,7 +1733,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -1681,7 +1744,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -1730,10 +1793,10 @@
         <v>82</v>
       </c>
       <c r="D52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1747,7 +1810,10 @@
         <v>84</v>
       </c>
       <c r="D53" t="s">
-        <v>192</v>
+        <v>191</v>
+      </c>
+      <c r="E53" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1761,10 +1827,10 @@
         <v>86</v>
       </c>
       <c r="D54" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" t="s">
         <v>193</v>
-      </c>
-      <c r="E54" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1778,7 +1844,10 @@
         <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>191</v>
+        <v>190</v>
+      </c>
+      <c r="E55" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1803,7 +1872,10 @@
         <v>92</v>
       </c>
       <c r="D57" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="E57" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1883,10 +1955,10 @@
         <v>102</v>
       </c>
       <c r="D64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -1900,10 +1972,10 @@
         <v>104</v>
       </c>
       <c r="D65" t="s">
+        <v>169</v>
+      </c>
+      <c r="E65" t="s">
         <v>170</v>
-      </c>
-      <c r="E65" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2028,10 +2100,10 @@
         <v>123</v>
       </c>
       <c r="D77" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2056,10 +2128,10 @@
         <v>127</v>
       </c>
       <c r="D79" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2192,10 +2264,10 @@
         <v>146</v>
       </c>
       <c r="D91" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E91" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2209,10 +2281,10 @@
         <v>148</v>
       </c>
       <c r="D92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E92" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2248,10 +2320,10 @@
         <v>154</v>
       </c>
       <c r="D95" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E95" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2265,10 +2337,10 @@
         <v>156</v>
       </c>
       <c r="D96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E96" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
corrected PCINT pin mapping
moved pretty much every interrupt pin to A8-A15, which had the secondary benefit of greatly reducing their trace length.
</commit_message>
<xml_diff>
--- a/Electronics/Low Level v3/Pin Mapping.xlsx
+++ b/Electronics/Low Level v3/Pin Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F535DA3-0721-434A-900B-D42314399404}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28A8BB6-29E7-FF48-896E-DE48F8AC78D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="21160" xr2:uid="{2E9AF3F1-2BA1-F14D-8C1F-E5BC4609F5C6}"/>
   </bookViews>
@@ -533,9 +533,6 @@
     <t>Arduino Pin Name</t>
   </si>
   <si>
-    <t>LLBV3 Pin Name</t>
-  </si>
-  <si>
     <t>RX3</t>
   </si>
   <si>
@@ -590,9 +587,6 @@
     <t>Steering header</t>
   </si>
   <si>
-    <t>E-STOP (INT)</t>
-  </si>
-  <si>
     <t>REGEN_ACTIVE</t>
   </si>
   <si>
@@ -672,6 +666,12 @@
   </si>
   <si>
     <t>X3, no purpose assgined</t>
+  </si>
+  <si>
+    <t>Second Draft LLBV3 Pin Name</t>
+  </si>
+  <si>
+    <t>E-stop (INT)</t>
   </si>
 </sst>
 </file>
@@ -737,7 +737,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -750,11 +760,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -778,6 +788,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -785,6 +825,24 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1108,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4080FD99-07AF-0640-A5AF-54DF0F777A9D}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1132,10 +1190,10 @@
         <v>166</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>167</v>
+        <v>212</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1148,12 +1206,6 @@
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E2" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1166,10 +1218,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1183,10 +1235,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" t="s">
         <v>172</v>
-      </c>
-      <c r="E4" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1209,10 +1261,10 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1226,10 +1278,10 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1242,12 +1294,6 @@
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
@@ -1342,10 +1388,10 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
+        <v>183</v>
+      </c>
+      <c r="E17" t="s">
         <v>184</v>
-      </c>
-      <c r="E17" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1358,12 +1404,6 @@
       <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D18" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
@@ -1375,12 +1415,6 @@
       <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" t="s">
-        <v>181</v>
-      </c>
-      <c r="E19" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
@@ -1393,10 +1427,10 @@
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1410,10 +1444,10 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1427,10 +1461,10 @@
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1444,10 +1478,10 @@
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1460,12 +1494,6 @@
       <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D24" t="s">
-        <v>177</v>
-      </c>
-      <c r="E24" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
@@ -1477,12 +1505,6 @@
       <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D25" t="s">
-        <v>178</v>
-      </c>
-      <c r="E25" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
@@ -1494,12 +1516,6 @@
       <c r="C26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D26" t="s">
-        <v>179</v>
-      </c>
-      <c r="E26" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
@@ -1511,12 +1527,6 @@
       <c r="C27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E27" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
@@ -1611,10 +1621,10 @@
         <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1628,10 +1638,10 @@
         <v>55</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1793,10 +1803,10 @@
         <v>82</v>
       </c>
       <c r="D52" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E52" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1810,10 +1820,10 @@
         <v>84</v>
       </c>
       <c r="D53" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E53" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1827,10 +1837,10 @@
         <v>86</v>
       </c>
       <c r="D54" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E54" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1844,10 +1854,10 @@
         <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E55" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1872,10 +1882,10 @@
         <v>92</v>
       </c>
       <c r="D57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1955,10 +1965,10 @@
         <v>102</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -1972,10 +1982,10 @@
         <v>104</v>
       </c>
       <c r="D65" t="s">
+        <v>168</v>
+      </c>
+      <c r="E65" t="s">
         <v>169</v>
-      </c>
-      <c r="E65" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2100,10 +2110,10 @@
         <v>123</v>
       </c>
       <c r="D77" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2128,10 +2138,10 @@
         <v>127</v>
       </c>
       <c r="D79" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E79" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2175,6 +2185,12 @@
       <c r="C83" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="D83" t="s">
+        <v>179</v>
+      </c>
+      <c r="E83" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
@@ -2186,6 +2202,12 @@
       <c r="C84" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="D84" t="s">
+        <v>178</v>
+      </c>
+      <c r="E84" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
@@ -2197,6 +2219,12 @@
       <c r="C85" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="D85" t="s">
+        <v>176</v>
+      </c>
+      <c r="E85" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
@@ -2208,6 +2236,12 @@
       <c r="C86" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="D86" t="s">
+        <v>177</v>
+      </c>
+      <c r="E86" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
@@ -2219,6 +2253,12 @@
       <c r="C87" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="D87" t="s">
+        <v>181</v>
+      </c>
+      <c r="E87" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
@@ -2230,6 +2270,12 @@
       <c r="C88" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D88" t="s">
+        <v>175</v>
+      </c>
+      <c r="E88" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
@@ -2241,6 +2287,12 @@
       <c r="C89" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="D89" t="s">
+        <v>213</v>
+      </c>
+      <c r="E89" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
@@ -2252,6 +2304,12 @@
       <c r="C90" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="D90" t="s">
+        <v>180</v>
+      </c>
+      <c r="E90" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
@@ -2264,10 +2322,10 @@
         <v>146</v>
       </c>
       <c r="D91" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E91" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2281,10 +2339,10 @@
         <v>148</v>
       </c>
       <c r="D92" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E92" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2320,10 +2378,10 @@
         <v>154</v>
       </c>
       <c r="D95" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E95" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2337,10 +2395,10 @@
         <v>156</v>
       </c>
       <c r="D96" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E96" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2399,24 +2457,30 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PCINT">
+  <conditionalFormatting sqref="A18:C19 A89:C90 A24:C27 A91:D1048576 A1:D17 A88:D88 A20:D23 A28:D81 A82:C87 D83:D1048576">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="PCINT">
       <formula>NOT(ISERROR(SEARCH("PCINT",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Digital Pin">
+  <conditionalFormatting sqref="A18:C19 A24:C27 A20:XFD23 A1:XFD1 A2:D2 F2:XFD2 F24:XFD27 A3:XFD7 A9:XFD17 A8:D8 F8:XFD8 F18:XFD19 A28:XFD81 I82:XFD82 F82 A82:C86 D83:XFD83 D84:F86 I84:XFD86 A87:XFD1048576">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="PWM">
+      <formula>NOT(ISERROR(SEARCH("PWM",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Digital Pin">
       <formula>NOT(ISERROR(SEARCH("Digital Pin",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PWM">
-      <formula>NOT(ISERROR(SEARCH("PWM",A1)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="INT">
+  <conditionalFormatting sqref="D1:D17 D20:D23 D28:D81 D83:D1048576">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="INT">
       <formula>NOT(ISERROR(SEARCH("INT",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Analog pin">
+      <formula>NOT(ISERROR(SEARCH("Analog pin",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>